<commit_message>
fix some company_id's in sample data
</commit_message>
<xml_diff>
--- a/app/data/InputFormat.xlsx
+++ b/app/data/InputFormat.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daanm\Documents\temp\SBTi\SBTi-DEV\app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\src\SBTi\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17835"/>
   </bookViews>
   <sheets>
     <sheet name="Fundemental data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="190">
   <si>
     <t>Required</t>
   </si>
@@ -1019,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3032,8 +3032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3544,6 +3544,9 @@
       <c r="B13" t="s">
         <v>53</v>
       </c>
+      <c r="C13" t="s">
+        <v>174</v>
+      </c>
       <c r="E13" t="s">
         <v>175</v>
       </c>
@@ -3582,6 +3585,9 @@
       <c r="B14" t="s">
         <v>55</v>
       </c>
+      <c r="C14" t="s">
+        <v>174</v>
+      </c>
       <c r="E14" t="s">
         <v>175</v>
       </c>
@@ -3620,6 +3626,9 @@
       <c r="B15" t="s">
         <v>58</v>
       </c>
+      <c r="C15" t="s">
+        <v>174</v>
+      </c>
       <c r="E15" t="s">
         <v>175</v>
       </c>
@@ -3658,6 +3667,9 @@
       <c r="B16" t="s">
         <v>60</v>
       </c>
+      <c r="C16" t="s">
+        <v>174</v>
+      </c>
       <c r="E16" t="s">
         <v>175</v>
       </c>
@@ -3696,6 +3708,9 @@
       <c r="B17" t="s">
         <v>62</v>
       </c>
+      <c r="C17" t="s">
+        <v>174</v>
+      </c>
       <c r="E17" t="s">
         <v>175</v>
       </c>
@@ -3734,6 +3749,9 @@
       <c r="B18" t="s">
         <v>65</v>
       </c>
+      <c r="C18" t="s">
+        <v>174</v>
+      </c>
       <c r="E18" t="s">
         <v>175</v>
       </c>
@@ -3772,6 +3790,9 @@
       <c r="B19" t="s">
         <v>67</v>
       </c>
+      <c r="C19" t="s">
+        <v>174</v>
+      </c>
       <c r="E19" t="s">
         <v>189</v>
       </c>
@@ -3807,6 +3828,9 @@
       <c r="B20" t="s">
         <v>69</v>
       </c>
+      <c r="C20" t="s">
+        <v>174</v>
+      </c>
       <c r="E20" t="s">
         <v>189</v>
       </c>
@@ -3842,6 +3866,9 @@
       <c r="B21" t="s">
         <v>71</v>
       </c>
+      <c r="C21" t="s">
+        <v>174</v>
+      </c>
       <c r="E21" t="s">
         <v>189</v>
       </c>
@@ -3877,6 +3904,9 @@
       <c r="B22" t="s">
         <v>74</v>
       </c>
+      <c r="C22" t="s">
+        <v>174</v>
+      </c>
       <c r="E22" t="s">
         <v>189</v>
       </c>
@@ -3912,6 +3942,9 @@
       <c r="B23" t="s">
         <v>77</v>
       </c>
+      <c r="C23" t="s">
+        <v>174</v>
+      </c>
       <c r="E23" t="s">
         <v>189</v>
       </c>
@@ -6317,6 +6350,12 @@
       <c r="E81" t="s">
         <v>178</v>
       </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
       <c r="H81">
         <v>0.9</v>
       </c>
@@ -6754,7 +6793,7 @@
         <v>59</v>
       </c>
       <c r="B92" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C92" t="s">
         <v>182</v>
@@ -7114,7 +7153,7 @@
         <v>31</v>
       </c>
       <c r="B101" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C101" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
fix more columns + ECOTS aggregation method
</commit_message>
<xml_diff>
--- a/app/data/InputFormat.xlsx
+++ b/app/data/InputFormat.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="189">
   <si>
     <t>Required</t>
   </si>
@@ -72,12 +72,6 @@
     <t>market_cap</t>
   </si>
   <si>
-    <t>enterprise_value</t>
-  </si>
-  <si>
-    <t>total_assets</t>
-  </si>
-  <si>
     <t>cash_equivalents</t>
   </si>
   <si>
@@ -588,13 +582,16 @@
     <t>Oil</t>
   </si>
   <si>
-    <t>Revenu</t>
-  </si>
-  <si>
     <t>company_id</t>
   </si>
   <si>
     <t>S3</t>
+  </si>
+  <si>
+    <t>company_enterprise_value</t>
+  </si>
+  <si>
+    <t>company_total_assets</t>
   </si>
 </sst>
 </file>
@@ -717,10 +714,10 @@
     <tableColumn id="6" name="sector"/>
     <tableColumn id="18" name="GHG_scope1+2"/>
     <tableColumn id="8" name="GHG_scope3"/>
-    <tableColumn id="9" name="Revenu"/>
+    <tableColumn id="9" name="Revenue"/>
     <tableColumn id="10" name="market_cap"/>
-    <tableColumn id="11" name="enterprise_value"/>
-    <tableColumn id="12" name="total_assets" dataDxfId="0">
+    <tableColumn id="11" name="company_enterprise_value"/>
+    <tableColumn id="12" name="company_total_assets" dataDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[market_cap]]*Q3</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" name="cash_equivalents"/>
@@ -1019,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,10 +1026,10 @@
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="11" width="21.5703125" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1066,7 +1063,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1099,36 +1096,36 @@
         <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="N2" t="s">
         <v>14</v>
       </c>
       <c r="O2" t="s">
+        <v>187</v>
+      </c>
+      <c r="P2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q2" t="s">
         <v>15</v>
-      </c>
-      <c r="P2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="J3" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
       </c>
       <c r="K3">
         <v>24965246.128183831</v>
@@ -1154,19 +1151,19 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>25</v>
       </c>
       <c r="K4">
         <v>1288468.9201645069</v>
@@ -1175,7 +1172,7 @@
         <v>1739806.6661840158</v>
       </c>
       <c r="M4">
-        <v>276185899.61435145</v>
+        <v>276185899.61435097</v>
       </c>
       <c r="N4">
         <v>170431377.0111033</v>
@@ -1192,19 +1189,19 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
+      <c r="J5" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
       </c>
       <c r="K5">
         <v>230191.46897492089</v>
@@ -1230,19 +1227,19 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
         <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
       </c>
       <c r="K6">
         <v>178705.06184309252</v>
@@ -1268,19 +1265,19 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K7">
         <v>97771.835813462851</v>
@@ -1306,19 +1303,19 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
         <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" t="s">
-        <v>39</v>
       </c>
       <c r="K8">
         <v>466041.10015869705</v>
@@ -1344,19 +1341,19 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K9">
         <v>128250.99022235045</v>
@@ -1382,19 +1379,19 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" t="s">
-        <v>44</v>
       </c>
       <c r="K10">
         <v>1736.1153986195452</v>
@@ -1420,19 +1417,19 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E11" t="s">
         <v>46</v>
       </c>
-      <c r="D11" t="s">
+      <c r="J11" t="s">
         <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J11" t="s">
-        <v>49</v>
       </c>
       <c r="K11">
         <v>196777.12553570265</v>
@@ -1458,19 +1455,19 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K12">
         <v>259165.86622702488</v>
@@ -1496,19 +1493,19 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K13">
         <v>81810.361536814045</v>
@@ -1534,19 +1531,19 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
         <v>54</v>
       </c>
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" t="s">
-        <v>56</v>
-      </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K14">
         <v>14847.919278129972</v>
@@ -1572,19 +1569,19 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K15">
         <v>31895.87194649009</v>
@@ -1610,19 +1607,19 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K16">
         <v>42305.282163536431</v>
@@ -1648,19 +1645,19 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
         <v>61</v>
       </c>
-      <c r="B17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" t="s">
-        <v>63</v>
-      </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K17">
         <v>118561.91297201814</v>
@@ -1686,19 +1683,19 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K18">
         <v>45833216.792469583</v>
@@ -1724,19 +1721,19 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K19">
         <v>9600.4773434214167</v>
@@ -1762,19 +1759,19 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K20">
         <v>25428190.928034011</v>
@@ -1786,7 +1783,7 @@
         <v>1236962789.3246891</v>
       </c>
       <c r="N20">
-        <v>938015347.69711757</v>
+        <v>938015347.69711804</v>
       </c>
       <c r="O20">
         <v>1252496335.1625824</v>
@@ -1800,19 +1797,19 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
         <v>70</v>
       </c>
-      <c r="B21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" t="s">
-        <v>72</v>
-      </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K21">
         <v>85293.345618346313</v>
@@ -1838,19 +1835,19 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
         <v>73</v>
       </c>
-      <c r="B22" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" t="s">
-        <v>75</v>
-      </c>
       <c r="E22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K22">
         <v>988.46631917228888</v>
@@ -1876,19 +1873,19 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
         <v>76</v>
       </c>
-      <c r="B23" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" t="s">
-        <v>78</v>
-      </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K23">
         <v>20210717.506183945</v>
@@ -1914,19 +1911,19 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K24">
         <v>2878524.2770361695</v>
@@ -1952,19 +1949,19 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K25">
         <v>589526.73014329805</v>
@@ -1990,19 +1987,19 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" t="s">
         <v>83</v>
       </c>
-      <c r="B26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" t="s">
-        <v>85</v>
-      </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K26">
         <v>7790.9166015573965</v>
@@ -2028,19 +2025,19 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K27">
         <v>2166428.3608621312</v>
@@ -2066,19 +2063,19 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" t="s">
         <v>88</v>
-      </c>
-      <c r="B28" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" t="s">
-        <v>48</v>
-      </c>
-      <c r="J28" t="s">
-        <v>90</v>
       </c>
       <c r="K28">
         <v>1374527.5713624337</v>
@@ -2104,19 +2101,19 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" t="s">
         <v>91</v>
       </c>
-      <c r="B29" t="s">
+      <c r="E29" t="s">
         <v>92</v>
       </c>
-      <c r="D29" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" t="s">
-        <v>94</v>
-      </c>
       <c r="J29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K29">
         <v>36340.85512554364</v>
@@ -2142,19 +2139,19 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" t="s">
+        <v>92</v>
+      </c>
+      <c r="J30" t="s">
         <v>95</v>
-      </c>
-      <c r="B30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J30" t="s">
-        <v>97</v>
       </c>
       <c r="K30">
         <v>68737.202118534289</v>
@@ -2180,19 +2177,19 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" t="s">
+        <v>92</v>
+      </c>
+      <c r="J31" t="s">
         <v>98</v>
-      </c>
-      <c r="B31" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" t="s">
-        <v>93</v>
-      </c>
-      <c r="E31" t="s">
-        <v>94</v>
-      </c>
-      <c r="J31" t="s">
-        <v>100</v>
       </c>
       <c r="K31">
         <v>100484.3202610756</v>
@@ -2218,19 +2215,19 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" t="s">
         <v>101</v>
       </c>
-      <c r="B32" t="s">
-        <v>102</v>
-      </c>
-      <c r="D32" t="s">
-        <v>103</v>
-      </c>
       <c r="E32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K32">
         <v>14088280.445939962</v>
@@ -2256,19 +2253,19 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K33">
         <v>118941.23272573021</v>
@@ -2294,19 +2291,19 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D34" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K34">
         <v>21988.936351392673</v>
@@ -2332,19 +2329,19 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E35" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K35">
         <v>11935572.900812317</v>
@@ -2370,19 +2367,19 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" t="s">
         <v>110</v>
       </c>
-      <c r="B36" t="s">
+      <c r="E36" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" t="s">
         <v>111</v>
-      </c>
-      <c r="D36" t="s">
-        <v>112</v>
-      </c>
-      <c r="E36" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" t="s">
-        <v>113</v>
       </c>
       <c r="K36">
         <v>2107.7428559933919</v>
@@ -2408,19 +2405,19 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K37">
         <v>314936.79875185777</v>
@@ -2446,19 +2443,19 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B38" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K38">
         <v>91117.578012331389</v>
@@ -2484,19 +2481,19 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" t="s">
         <v>118</v>
-      </c>
-      <c r="B39" t="s">
-        <v>119</v>
-      </c>
-      <c r="D39" t="s">
-        <v>112</v>
-      </c>
-      <c r="E39" t="s">
-        <v>21</v>
-      </c>
-      <c r="J39" t="s">
-        <v>120</v>
       </c>
       <c r="K39">
         <v>26.865407941423623</v>
@@ -2522,19 +2519,19 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E40" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K40">
         <v>1988.9893256430512</v>
@@ -2560,19 +2557,19 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E41" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K41">
         <v>116613.16602106349</v>
@@ -2598,19 +2595,19 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B42" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D42" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E42" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K42">
         <v>2641303.9499925142</v>
@@ -2636,19 +2633,19 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" t="s">
         <v>127</v>
       </c>
-      <c r="B43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D43" t="s">
-        <v>129</v>
-      </c>
       <c r="E43" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K43">
         <v>34886.045315286356</v>
@@ -2674,19 +2671,19 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" t="s">
         <v>130</v>
       </c>
-      <c r="B44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D44" t="s">
-        <v>132</v>
-      </c>
       <c r="E44" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J44" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K44">
         <v>13266889.881567331</v>
@@ -2712,19 +2709,19 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B45" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D45" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E45" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J45" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K45">
         <v>1436916.8962362793</v>
@@ -2750,19 +2747,19 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" t="s">
+        <v>134</v>
+      </c>
+      <c r="D46" t="s">
         <v>135</v>
       </c>
-      <c r="B46" t="s">
-        <v>136</v>
-      </c>
-      <c r="D46" t="s">
-        <v>137</v>
-      </c>
       <c r="E46" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J46" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K46">
         <v>6611043.5529440343</v>
@@ -2788,19 +2785,19 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" t="s">
         <v>138</v>
       </c>
-      <c r="B47" t="s">
-        <v>139</v>
-      </c>
-      <c r="D47" t="s">
-        <v>140</v>
-      </c>
       <c r="E47" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J47" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K47">
         <v>8307064.9522866216</v>
@@ -2826,19 +2823,19 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" t="s">
+        <v>140</v>
+      </c>
+      <c r="D48" t="s">
         <v>141</v>
       </c>
-      <c r="B48" t="s">
+      <c r="E48" t="s">
         <v>142</v>
       </c>
-      <c r="D48" t="s">
-        <v>143</v>
-      </c>
-      <c r="E48" t="s">
-        <v>144</v>
-      </c>
       <c r="J48" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K48">
         <v>6086.1963717252083</v>
@@ -2864,19 +2861,19 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" t="s">
         <v>145</v>
       </c>
-      <c r="B49" t="s">
-        <v>146</v>
-      </c>
-      <c r="D49" t="s">
-        <v>147</v>
-      </c>
       <c r="E49" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J49" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K49">
         <v>121886.58843968091</v>
@@ -2902,19 +2899,19 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" t="s">
         <v>148</v>
       </c>
-      <c r="B50" t="s">
-        <v>149</v>
-      </c>
-      <c r="D50" t="s">
-        <v>150</v>
-      </c>
       <c r="E50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J50" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K50">
         <v>3073484.0384656894</v>
@@ -2940,19 +2937,19 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>149</v>
+      </c>
+      <c r="B51" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" t="s">
         <v>151</v>
       </c>
-      <c r="B51" t="s">
-        <v>152</v>
-      </c>
-      <c r="D51" t="s">
-        <v>153</v>
-      </c>
       <c r="E51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J51" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K51">
         <v>244176.80273373649</v>
@@ -2978,19 +2975,19 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" t="s">
         <v>154</v>
       </c>
-      <c r="B52" t="s">
+      <c r="E52" t="s">
         <v>155</v>
       </c>
-      <c r="D52" t="s">
-        <v>156</v>
-      </c>
-      <c r="E52" t="s">
-        <v>157</v>
-      </c>
       <c r="J52" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K52">
         <v>240504.60431777878</v>
@@ -3067,10 +3064,10 @@
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
       <c r="L1" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N1" s="10"/>
       <c r="O1" s="10"/>
@@ -3081,63 +3078,63 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
         <v>160</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>161</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>162</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>163</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>164</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>165</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>166</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>167</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>168</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>169</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>170</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>171</v>
-      </c>
-      <c r="O2" t="s">
-        <v>172</v>
-      </c>
-      <c r="P2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -3169,16 +3166,16 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -3211,16 +3208,16 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H5">
         <v>0.6</v>
@@ -3249,16 +3246,16 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" t="s">
         <v>176</v>
-      </c>
-      <c r="E6" t="s">
-        <v>178</v>
       </c>
       <c r="F6">
         <v>0.95</v>
@@ -3293,16 +3290,16 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" t="s">
         <v>176</v>
-      </c>
-      <c r="E7" t="s">
-        <v>178</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -3337,16 +3334,16 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -3378,16 +3375,16 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H9">
         <v>0.8</v>
@@ -3416,16 +3413,16 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -3457,16 +3454,16 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -3498,16 +3495,16 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -3539,16 +3536,16 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -3580,16 +3577,16 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -3621,16 +3618,16 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -3662,16 +3659,16 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -3703,16 +3700,16 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E17" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -3744,16 +3741,16 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -3785,16 +3782,16 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E19" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H19">
         <v>0.12</v>
@@ -3823,16 +3820,16 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H20">
         <v>0.3</v>
@@ -3861,16 +3858,16 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E21" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H21">
         <v>0.4</v>
@@ -3899,16 +3896,16 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E22" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H22">
         <v>0.5</v>
@@ -3937,16 +3934,16 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E23" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H23">
         <v>0.6</v>
@@ -3975,16 +3972,16 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E24" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H24">
         <v>0.8</v>
@@ -4013,19 +4010,19 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E25" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H25">
         <v>0.7</v>
@@ -4054,16 +4051,16 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -4095,16 +4092,16 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E27" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -4136,19 +4133,19 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F28">
         <v>0.95</v>
@@ -4180,19 +4177,19 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D29" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E29" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H29">
         <v>0.8</v>
@@ -4215,19 +4212,19 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E30" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H30">
         <v>0.9</v>
@@ -4256,16 +4253,16 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F31">
         <v>0.99</v>
@@ -4297,19 +4294,19 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D32" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E32" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H32">
         <v>0.81</v>
@@ -4338,16 +4335,16 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E33" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F33">
         <v>0.85</v>
@@ -4379,16 +4376,16 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E34" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -4417,19 +4414,19 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D35" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E35" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -4458,16 +4455,16 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -4493,16 +4490,16 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C37" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -4534,19 +4531,19 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E38" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H38">
         <v>0.159</v>
@@ -4575,19 +4572,19 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D39" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E39" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H39">
         <v>0.75</v>
@@ -4616,16 +4613,16 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E40" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -4654,19 +4651,19 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D41" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E41" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F41">
         <v>0.71</v>
@@ -4692,19 +4689,19 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D42" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F42">
         <v>0.75</v>
@@ -4736,19 +4733,19 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D43" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E43" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -4780,16 +4777,16 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C44" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E44" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -4821,16 +4818,16 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C45" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E45" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F45">
         <v>0.86</v>
@@ -4862,16 +4859,16 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F46">
         <v>0.86</v>
@@ -4903,19 +4900,19 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C47" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D47" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E47" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -4947,19 +4944,19 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C48" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D48" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E48" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -4991,16 +4988,16 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B49" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C49" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E49" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F49">
         <v>0.65</v>
@@ -5032,19 +5029,19 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C50" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D50" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E50" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F50">
         <v>0.65</v>
@@ -5076,19 +5073,19 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C51" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D51" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E51" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F51">
         <v>0.65</v>
@@ -5123,16 +5120,16 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E52" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -5164,19 +5161,19 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C53" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D53" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E53" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -5205,19 +5202,19 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D54" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E54" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -5249,16 +5246,16 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E55" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F55">
         <v>0.7</v>
@@ -5290,16 +5287,16 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C56" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E56" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -5331,16 +5328,16 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E57" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -5372,16 +5369,16 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C58" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E58" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F58">
         <v>0.97</v>
@@ -5413,16 +5410,16 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C59" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E59" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -5454,19 +5451,19 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C60" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D60" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E60" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -5498,19 +5495,19 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C61" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D61" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E61" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F61">
         <v>0.75</v>
@@ -5542,19 +5539,19 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C62" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D62" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E62" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -5586,16 +5583,16 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B63" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C63" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E63" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -5627,16 +5624,16 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B64" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C64" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E64" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -5668,16 +5665,16 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B65" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C65" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E65" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F65">
         <v>0.95</v>
@@ -5709,19 +5706,19 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C66" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D66" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E66" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F66">
         <v>0.95</v>
@@ -5753,19 +5750,19 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B67" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C67" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D67" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E67" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F67">
         <v>0.93</v>
@@ -5797,16 +5794,16 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B68" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C68" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E68" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -5838,19 +5835,19 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B69" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C69" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D69" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E69" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -5882,16 +5879,16 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B70" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C70" t="s">
+        <v>180</v>
+      </c>
+      <c r="E70" t="s">
         <v>182</v>
-      </c>
-      <c r="E70" t="s">
-        <v>184</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -5920,16 +5917,16 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B71" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C71" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E71" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -5961,19 +5958,19 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B72" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C72" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D72" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E72" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -6005,19 +6002,19 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B73" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C73" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D73" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E73" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H73">
         <v>0.7</v>
@@ -6046,16 +6043,16 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B74" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C74" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E74" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -6087,19 +6084,19 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B75" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C75" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D75" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E75" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -6131,16 +6128,16 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B76" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C76" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E76" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -6172,16 +6169,16 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B77" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C77" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E77" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -6213,16 +6210,16 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C78" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E78" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -6254,19 +6251,19 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B79" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D79" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E79" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -6298,16 +6295,16 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C80" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E80" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H80">
         <v>0.95</v>
@@ -6336,19 +6333,19 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B81" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C81" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D81" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E81" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -6383,19 +6380,19 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B82" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C82" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D82" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E82" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -6427,19 +6424,19 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B83" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C83" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D83" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E83" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -6468,19 +6465,19 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B84" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C84" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D84" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E84" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H84">
         <v>0.6</v>
@@ -6509,19 +6506,19 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B85" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C85" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D85" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E85" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H85">
         <v>0.95</v>
@@ -6550,16 +6547,16 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B86" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C86" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E86" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F86">
         <v>1</v>
@@ -6591,16 +6588,16 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B87" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C87" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E87" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H87">
         <v>0.89270000000000005</v>
@@ -6629,19 +6626,19 @@
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B88" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C88" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D88" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E88" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F88">
         <v>0.93100000000000005</v>
@@ -6673,16 +6670,16 @@
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B89" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C89" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E89" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G89">
         <v>0.04</v>
@@ -6711,16 +6708,16 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B90" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C90" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E90" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G90">
         <v>1</v>
@@ -6749,19 +6746,19 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B91" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C91" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D91" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E91" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G91">
         <v>0.7</v>
@@ -6790,16 +6787,16 @@
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B92" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C92" t="s">
+        <v>180</v>
+      </c>
+      <c r="E92" t="s">
         <v>182</v>
-      </c>
-      <c r="E92" t="s">
-        <v>184</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -6828,16 +6825,16 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B93" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C93" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E93" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G93">
         <v>1</v>
@@ -6866,16 +6863,16 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B94" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C94" t="s">
+        <v>180</v>
+      </c>
+      <c r="E94" t="s">
         <v>182</v>
-      </c>
-      <c r="E94" t="s">
-        <v>184</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -6904,16 +6901,16 @@
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B95" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C95" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E95" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G95">
         <v>1</v>
@@ -6942,16 +6939,16 @@
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B96" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C96" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E96" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -6983,16 +6980,16 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B97" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C97" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E97" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -7024,19 +7021,19 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B98" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C98" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D98" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E98" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -7068,19 +7065,19 @@
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B99" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C99" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D99" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E99" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F99">
         <v>1</v>
@@ -7112,16 +7109,16 @@
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B100" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C100" t="s">
+        <v>180</v>
+      </c>
+      <c r="E100" t="s">
         <v>182</v>
-      </c>
-      <c r="E100" t="s">
-        <v>184</v>
       </c>
       <c r="F100">
         <v>1</v>
@@ -7150,16 +7147,16 @@
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B101" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C101" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E101" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G101">
         <v>1</v>
@@ -7188,19 +7185,19 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B102" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C102" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D102" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E102" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F102">
         <v>0.87</v>
@@ -7232,16 +7229,16 @@
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B103" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C103" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E103" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H103">
         <v>1</v>
@@ -7270,16 +7267,16 @@
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B104" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C104" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E104" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F104">
         <v>0.27</v>
@@ -7311,19 +7308,19 @@
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B105" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C105" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D105" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E105" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -7355,19 +7352,19 @@
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B106" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C106" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D106" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E106" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -7399,19 +7396,19 @@
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B107" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C107" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D107" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E107" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H107">
         <v>0.44</v>
@@ -7440,19 +7437,19 @@
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B108" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C108" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D108" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E108" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F108">
         <v>1</v>
@@ -7484,16 +7481,16 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B109" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C109" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E109" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F109">
         <v>0.94</v>
@@ -7525,16 +7522,16 @@
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B110" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C110" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E110" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F110">
         <v>0.94</v>
@@ -7566,19 +7563,19 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B111" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C111" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D111" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E111" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F111">
         <v>0.94</v>
@@ -7610,19 +7607,19 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B112" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C112" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D112" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E112" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H112">
         <v>1</v>
@@ -7651,19 +7648,19 @@
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B113" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C113" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D113" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E113" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F113">
         <v>0.99</v>
@@ -7692,16 +7689,16 @@
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C114" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E114" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F114">
         <v>1</v>
@@ -7733,19 +7730,19 @@
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B115" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C115" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D115" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E115" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H115">
         <v>1</v>
@@ -7774,16 +7771,16 @@
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B116" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C116" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E116" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F116">
         <v>0.99</v>
@@ -7815,16 +7812,16 @@
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B117" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C117" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E117" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -7856,16 +7853,16 @@
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B118" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C118" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E118" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F118">
         <v>0.66839999999999999</v>
@@ -7897,19 +7894,19 @@
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B119" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C119" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D119" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E119" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F119">
         <v>0.2024</v>
@@ -7941,19 +7938,19 @@
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B120" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C120" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D120" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E120" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F120">
         <v>0.66900000000000004</v>
@@ -7985,16 +7982,16 @@
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B121" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C121" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E121" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F121">
         <v>1</v>
@@ -8026,19 +8023,19 @@
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B122" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C122" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D122" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E122" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F122">
         <v>0.6</v>

</xml_diff>

<commit_message>
fix typo in excel tab 'fundemental data' ==> 'fundamental data'
</commit_message>
<xml_diff>
--- a/app/data/InputFormat.xlsx
+++ b/app/data/InputFormat.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="Fundemental data" sheetId="1" r:id="rId1"/>
+    <sheet name="Fundamental data" sheetId="1" r:id="rId1"/>
     <sheet name="Target data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="189">
   <si>
     <t>Required</t>
   </si>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3030,7 +3030,7 @@
   <dimension ref="A1:Q122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3174,6 +3174,9 @@
       <c r="C4" t="s">
         <v>174</v>
       </c>
+      <c r="D4" t="s">
+        <v>179</v>
+      </c>
       <c r="E4" t="s">
         <v>175</v>
       </c>
@@ -3216,6 +3219,9 @@
       <c r="C5" t="s">
         <v>174</v>
       </c>
+      <c r="D5" t="s">
+        <v>179</v>
+      </c>
       <c r="E5" t="s">
         <v>186</v>
       </c>
@@ -3254,6 +3260,9 @@
       <c r="C6" t="s">
         <v>174</v>
       </c>
+      <c r="D6" t="s">
+        <v>179</v>
+      </c>
       <c r="E6" t="s">
         <v>176</v>
       </c>
@@ -3298,6 +3307,9 @@
       <c r="C7" t="s">
         <v>174</v>
       </c>
+      <c r="D7" t="s">
+        <v>179</v>
+      </c>
       <c r="E7" t="s">
         <v>176</v>
       </c>
@@ -3342,6 +3354,9 @@
       <c r="C8" t="s">
         <v>174</v>
       </c>
+      <c r="D8" t="s">
+        <v>179</v>
+      </c>
       <c r="E8" t="s">
         <v>173</v>
       </c>
@@ -3421,6 +3436,9 @@
       <c r="C10" t="s">
         <v>174</v>
       </c>
+      <c r="D10" t="s">
+        <v>179</v>
+      </c>
       <c r="E10" t="s">
         <v>173</v>
       </c>
@@ -3462,6 +3480,9 @@
       <c r="C11" t="s">
         <v>174</v>
       </c>
+      <c r="D11" t="s">
+        <v>179</v>
+      </c>
       <c r="E11" t="s">
         <v>173</v>
       </c>
@@ -3503,6 +3524,9 @@
       <c r="C12" t="s">
         <v>174</v>
       </c>
+      <c r="D12" t="s">
+        <v>179</v>
+      </c>
       <c r="E12" t="s">
         <v>173</v>
       </c>
@@ -6177,6 +6201,9 @@
       <c r="C77" t="s">
         <v>178</v>
       </c>
+      <c r="D77" t="s">
+        <v>179</v>
+      </c>
       <c r="E77" t="s">
         <v>173</v>
       </c>
@@ -6217,6 +6244,9 @@
       </c>
       <c r="C78" t="s">
         <v>178</v>
+      </c>
+      <c r="D78" t="s">
+        <v>179</v>
       </c>
       <c r="E78" t="s">
         <v>173</v>

</xml_diff>

<commit_message>
use percentage instead of decimal value for annual reduction rate in temperature score calculation
</commit_message>
<xml_diff>
--- a/app/data/InputFormat.xlsx
+++ b/app/data/InputFormat.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fundamental data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="189">
   <si>
     <t>Required</t>
   </si>
@@ -727,8 +727,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table4" displayName="Table4" ref="A2:P122" totalsRowShown="0">
-  <autoFilter ref="A2:P122"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table4" displayName="Table4" ref="A2:P121" totalsRowShown="0">
+  <autoFilter ref="A2:P121"/>
   <tableColumns count="16">
     <tableColumn id="1" name="company_name"/>
     <tableColumn id="2" name="company_id"/>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3027,10 +3027,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q122"/>
+  <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3566,7 +3566,7 @@
         <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E13" t="s">
         <v>173</v>
@@ -3578,7 +3578,7 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <v>2017</v>
@@ -5288,13 +5288,13 @@
         <v>0.7</v>
       </c>
       <c r="I55">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="J55">
         <v>2015</v>
       </c>
       <c r="K55">
-        <v>2020</v>
+        <v>2033</v>
       </c>
       <c r="L55">
         <v>2015</v>
@@ -6738,69 +6738,69 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B90" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C90" t="s">
-        <v>180</v>
+        <v>178</v>
+      </c>
+      <c r="D90" t="s">
+        <v>179</v>
       </c>
       <c r="E90" t="s">
         <v>175</v>
       </c>
       <c r="G90">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="I90">
-        <v>0.41000000000000003</v>
+        <v>0.63</v>
       </c>
       <c r="J90">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="K90">
-        <v>2018</v>
+        <v>2030</v>
       </c>
       <c r="L90">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="M90">
-        <v>21032.177657544897</v>
+        <v>0</v>
       </c>
       <c r="N90">
-        <v>7567.8223424551024</v>
+        <v>0</v>
       </c>
       <c r="P90">
-        <v>0.23600000000000002</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B91" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C91" t="s">
-        <v>178</v>
-      </c>
-      <c r="D91" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E91" t="s">
-        <v>175</v>
-      </c>
-      <c r="G91">
-        <v>0.7</v>
+        <v>182</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
       </c>
       <c r="I91">
-        <v>0.63</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="J91">
         <v>2010</v>
       </c>
       <c r="K91">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="L91">
         <v>2015</v>
@@ -6812,7 +6812,7 @@
         <v>0</v>
       </c>
       <c r="P91">
-        <v>0.93</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -6826,28 +6826,28 @@
         <v>180</v>
       </c>
       <c r="E92" t="s">
-        <v>182</v>
-      </c>
-      <c r="F92">
+        <v>175</v>
+      </c>
+      <c r="G92">
         <v>1</v>
       </c>
       <c r="I92">
-        <v>0.57000000000000006</v>
+        <v>0.23</v>
       </c>
       <c r="J92">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="K92">
-        <v>2050</v>
+        <v>2019</v>
       </c>
       <c r="L92">
         <v>2015</v>
       </c>
       <c r="M92">
-        <v>0</v>
+        <v>86188.973721744012</v>
       </c>
       <c r="N92">
-        <v>0</v>
+        <v>24078.026278255991</v>
       </c>
       <c r="P92">
         <v>1</v>
@@ -6855,25 +6855,25 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B93" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C93" t="s">
         <v>180</v>
       </c>
       <c r="E93" t="s">
-        <v>175</v>
-      </c>
-      <c r="G93">
+        <v>182</v>
+      </c>
+      <c r="F93">
         <v>1</v>
       </c>
       <c r="I93">
-        <v>0.23</v>
+        <v>0.52</v>
       </c>
       <c r="J93">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="K93">
         <v>2019</v>
@@ -6882,10 +6882,10 @@
         <v>2015</v>
       </c>
       <c r="M93">
-        <v>86188.973721744012</v>
+        <v>157300.227918088</v>
       </c>
       <c r="N93">
-        <v>24078.026278255991</v>
+        <v>256065.772081912</v>
       </c>
       <c r="P93">
         <v>1</v>
@@ -6902,77 +6902,80 @@
         <v>180</v>
       </c>
       <c r="E94" t="s">
-        <v>182</v>
-      </c>
-      <c r="F94">
+        <v>175</v>
+      </c>
+      <c r="G94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>0.52</v>
+        <v>0.71</v>
       </c>
       <c r="J94">
-        <v>2006</v>
+        <v>2017</v>
       </c>
       <c r="K94">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="L94">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="M94">
-        <v>157300.227918088</v>
+        <v>76119.155977881208</v>
       </c>
       <c r="N94">
-        <v>256065.772081912</v>
+        <v>34147.844022118792</v>
       </c>
       <c r="P94">
-        <v>1</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B95" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C95" t="s">
         <v>180</v>
       </c>
       <c r="E95" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
       </c>
       <c r="G95">
         <v>1</v>
       </c>
       <c r="I95">
-        <v>0.71</v>
+        <v>0.66</v>
       </c>
       <c r="J95">
-        <v>2017</v>
+        <v>2005</v>
       </c>
       <c r="K95">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="L95">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="M95">
-        <v>76119.155977881208</v>
+        <v>50287.328437504606</v>
       </c>
       <c r="N95">
-        <v>34147.844022118792</v>
+        <v>363078.67156249541</v>
       </c>
       <c r="P95">
-        <v>0.13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="B96" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="C96" t="s">
         <v>180</v>
@@ -6987,36 +6990,39 @@
         <v>1</v>
       </c>
       <c r="I96">
-        <v>0.66</v>
+        <v>0.3</v>
       </c>
       <c r="J96">
-        <v>2005</v>
+        <v>2015</v>
       </c>
       <c r="K96">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="L96">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="M96">
-        <v>50287.328437504606</v>
+        <v>220221.12183529223</v>
       </c>
       <c r="N96">
-        <v>363078.67156249541</v>
+        <v>310630.27816470782</v>
       </c>
       <c r="P96">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B97" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C97" t="s">
-        <v>180</v>
+        <v>178</v>
+      </c>
+      <c r="D97" t="s">
+        <v>179</v>
       </c>
       <c r="E97" t="s">
         <v>173</v>
@@ -7028,22 +7034,22 @@
         <v>1</v>
       </c>
       <c r="I97">
-        <v>0.3</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="J97">
-        <v>2015</v>
+        <v>2008</v>
       </c>
       <c r="K97">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="L97">
         <v>2015</v>
       </c>
       <c r="M97">
-        <v>220221.12183529223</v>
+        <v>152767.86090478685</v>
       </c>
       <c r="N97">
-        <v>310630.27816470782</v>
+        <v>378083.53909521317</v>
       </c>
       <c r="P97">
         <v>0</v>
@@ -7051,10 +7057,10 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B98" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C98" t="s">
         <v>178</v>
@@ -7072,66 +7078,60 @@
         <v>1</v>
       </c>
       <c r="I98">
-        <v>0.57999999999999996</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="J98">
-        <v>2008</v>
+        <v>2013</v>
       </c>
       <c r="K98">
         <v>2030</v>
       </c>
       <c r="L98">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="M98">
-        <v>152767.86090478685</v>
+        <v>523303.09094109439</v>
       </c>
       <c r="N98">
-        <v>378083.53909521317</v>
+        <v>7548.309058905611</v>
       </c>
       <c r="P98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B99" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C99" t="s">
-        <v>178</v>
-      </c>
-      <c r="D99" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E99" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="F99">
         <v>1</v>
       </c>
-      <c r="G99">
-        <v>1</v>
-      </c>
       <c r="I99">
-        <v>0.57000000000000006</v>
+        <v>0.38</v>
       </c>
       <c r="J99">
         <v>2013</v>
       </c>
       <c r="K99">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="L99">
-        <v>2013</v>
+        <v>2017</v>
       </c>
       <c r="M99">
-        <v>523303.09094109439</v>
+        <v>388368.40900136431</v>
       </c>
       <c r="N99">
-        <v>7548.309058905611</v>
+        <v>142482.99099863574</v>
       </c>
       <c r="P99">
         <v>1</v>
@@ -7148,51 +7148,57 @@
         <v>180</v>
       </c>
       <c r="E100" t="s">
-        <v>182</v>
-      </c>
-      <c r="F100">
+        <v>175</v>
+      </c>
+      <c r="G100">
         <v>1</v>
       </c>
       <c r="I100">
-        <v>0.38</v>
+        <v>1</v>
       </c>
       <c r="J100">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="K100">
-        <v>2050</v>
+        <v>2020</v>
       </c>
       <c r="L100">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="M100">
-        <v>388368.40900136431</v>
+        <v>19905.125464660872</v>
       </c>
       <c r="N100">
-        <v>142482.99099863574</v>
+        <v>18145.874535339128</v>
       </c>
       <c r="P100">
-        <v>1</v>
+        <v>0.82000000000000006</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B101" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C101" t="s">
-        <v>180</v>
+        <v>178</v>
+      </c>
+      <c r="D101" t="s">
+        <v>179</v>
       </c>
       <c r="E101" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+      <c r="F101">
+        <v>0.87</v>
       </c>
       <c r="G101">
-        <v>1</v>
+        <v>0.87</v>
       </c>
       <c r="I101">
-        <v>1</v>
+        <v>0.63</v>
       </c>
       <c r="J101">
         <v>2011</v>
@@ -7204,54 +7210,48 @@
         <v>2016</v>
       </c>
       <c r="M101">
-        <v>19905.125464660872</v>
+        <v>133558.90949356617</v>
       </c>
       <c r="N101">
-        <v>18145.874535339128</v>
+        <v>85549.090506433844</v>
       </c>
       <c r="P101">
-        <v>0.82000000000000006</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B102" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C102" t="s">
         <v>178</v>
       </c>
-      <c r="D102" t="s">
-        <v>179</v>
-      </c>
       <c r="E102" t="s">
-        <v>173</v>
-      </c>
-      <c r="F102">
-        <v>0.87</v>
-      </c>
-      <c r="G102">
-        <v>0.87</v>
+        <v>186</v>
+      </c>
+      <c r="H102">
+        <v>1</v>
       </c>
       <c r="I102">
-        <v>0.63</v>
+        <v>0.79</v>
       </c>
       <c r="J102">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="K102">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="L102">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="M102">
-        <v>133558.90949356617</v>
+        <v>103544.86251166406</v>
       </c>
       <c r="N102">
-        <v>85549.090506433844</v>
+        <v>153614.13748833592</v>
       </c>
       <c r="P102">
         <v>1</v>
@@ -7259,22 +7259,25 @@
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B103" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C103" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E103" t="s">
-        <v>186</v>
-      </c>
-      <c r="H103">
-        <v>1</v>
+        <v>173</v>
+      </c>
+      <c r="F103">
+        <v>0.27</v>
+      </c>
+      <c r="G103">
+        <v>0.27</v>
       </c>
       <c r="I103">
-        <v>0.79</v>
+        <v>0.68</v>
       </c>
       <c r="J103">
         <v>2016</v>
@@ -7286,10 +7289,10 @@
         <v>2017</v>
       </c>
       <c r="M103">
-        <v>103544.86251166406</v>
+        <v>0</v>
       </c>
       <c r="N103">
-        <v>153614.13748833592</v>
+        <v>0</v>
       </c>
       <c r="P103">
         <v>1</v>
@@ -7297,25 +7300,28 @@
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B104" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C104" t="s">
-        <v>180</v>
+        <v>178</v>
+      </c>
+      <c r="D104" t="s">
+        <v>179</v>
       </c>
       <c r="E104" t="s">
         <v>173</v>
       </c>
       <c r="F104">
-        <v>0.27</v>
+        <v>1</v>
       </c>
       <c r="G104">
-        <v>0.27</v>
+        <v>1</v>
       </c>
       <c r="I104">
-        <v>0.68</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J104">
         <v>2016</v>
@@ -7333,15 +7339,15 @@
         <v>0</v>
       </c>
       <c r="P104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B105" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C105" t="s">
         <v>178</v>
@@ -7359,7 +7365,7 @@
         <v>1</v>
       </c>
       <c r="I105">
-        <v>0.28999999999999998</v>
+        <v>0.64</v>
       </c>
       <c r="J105">
         <v>2016</v>
@@ -7377,15 +7383,15 @@
         <v>0</v>
       </c>
       <c r="P105">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B106" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C106" t="s">
         <v>178</v>
@@ -7394,42 +7400,39 @@
         <v>179</v>
       </c>
       <c r="E106" t="s">
-        <v>173</v>
-      </c>
-      <c r="F106">
-        <v>1</v>
-      </c>
-      <c r="G106">
-        <v>1</v>
+        <v>186</v>
+      </c>
+      <c r="H106">
+        <v>0.44</v>
       </c>
       <c r="I106">
-        <v>0.64</v>
+        <v>0.45</v>
       </c>
       <c r="J106">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="K106">
-        <v>2019</v>
+        <v>2030</v>
       </c>
       <c r="L106">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="M106">
-        <v>0</v>
+        <v>248965.63534281132</v>
       </c>
       <c r="N106">
-        <v>0</v>
+        <v>32411.364657188678</v>
       </c>
       <c r="P106">
-        <v>7.0000000000000007E-2</v>
+        <v>0.70000000000000007</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B107" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C107" t="s">
         <v>178</v>
@@ -7438,16 +7441,19 @@
         <v>179</v>
       </c>
       <c r="E107" t="s">
-        <v>186</v>
-      </c>
-      <c r="H107">
-        <v>0.44</v>
+        <v>173</v>
+      </c>
+      <c r="F107">
+        <v>1</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
       </c>
       <c r="I107">
-        <v>0.45</v>
+        <v>0.65</v>
       </c>
       <c r="J107">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="K107">
         <v>2030</v>
@@ -7456,65 +7462,62 @@
         <v>2015</v>
       </c>
       <c r="M107">
-        <v>248965.63534281132</v>
+        <v>0</v>
       </c>
       <c r="N107">
-        <v>32411.364657188678</v>
+        <v>0</v>
       </c>
       <c r="P107">
-        <v>0.70000000000000007</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B108" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C108" t="s">
-        <v>178</v>
-      </c>
-      <c r="D108" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E108" t="s">
         <v>173</v>
       </c>
       <c r="F108">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="G108">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="I108">
-        <v>0.65</v>
+        <v>0.27</v>
       </c>
       <c r="J108">
-        <v>2010</v>
+        <v>2000</v>
       </c>
       <c r="K108">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="L108">
         <v>2015</v>
       </c>
       <c r="M108">
-        <v>0</v>
+        <v>542898.8931382685</v>
       </c>
       <c r="N108">
-        <v>0</v>
+        <v>903665.1068617315</v>
       </c>
       <c r="P108">
-        <v>0.61</v>
+        <v>0.69000000000000006</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B109" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C109" t="s">
         <v>180</v>
@@ -7529,36 +7532,39 @@
         <v>0.94</v>
       </c>
       <c r="I109">
-        <v>0.27</v>
+        <v>0.54</v>
       </c>
       <c r="J109">
         <v>2000</v>
       </c>
       <c r="K109">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="L109">
         <v>2015</v>
       </c>
       <c r="M109">
-        <v>542898.8931382685</v>
+        <v>1738037.0663147885</v>
       </c>
       <c r="N109">
-        <v>903665.1068617315</v>
+        <v>2019021.9336852115</v>
       </c>
       <c r="P109">
-        <v>0.69000000000000006</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B110" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C110" t="s">
-        <v>180</v>
+        <v>178</v>
+      </c>
+      <c r="D110" t="s">
+        <v>179</v>
       </c>
       <c r="E110" t="s">
         <v>173</v>
@@ -7570,33 +7576,33 @@
         <v>0.94</v>
       </c>
       <c r="I110">
-        <v>0.54</v>
+        <v>0.43</v>
       </c>
       <c r="J110">
-        <v>2000</v>
+        <v>2010</v>
       </c>
       <c r="K110">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="L110">
         <v>2015</v>
       </c>
       <c r="M110">
-        <v>1738037.0663147885</v>
+        <v>1353813.9178252162</v>
       </c>
       <c r="N110">
-        <v>2019021.9336852115</v>
+        <v>2403245.0821747836</v>
       </c>
       <c r="P110">
-        <v>0.55000000000000004</v>
+        <v>0.57020000000000004</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B111" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C111" t="s">
         <v>178</v>
@@ -7605,66 +7611,63 @@
         <v>179</v>
       </c>
       <c r="E111" t="s">
-        <v>173</v>
-      </c>
-      <c r="F111">
-        <v>0.94</v>
-      </c>
-      <c r="G111">
-        <v>0.94</v>
+        <v>186</v>
+      </c>
+      <c r="H111">
+        <v>1</v>
       </c>
       <c r="I111">
-        <v>0.43</v>
+        <v>0.62</v>
       </c>
       <c r="J111">
         <v>2010</v>
       </c>
       <c r="K111">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="L111">
         <v>2015</v>
       </c>
       <c r="M111">
-        <v>1353813.9178252162</v>
+        <v>0</v>
       </c>
       <c r="N111">
-        <v>2403245.0821747836</v>
+        <v>0</v>
       </c>
       <c r="P111">
-        <v>0.57020000000000004</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B112" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C112" t="s">
         <v>178</v>
       </c>
       <c r="D112" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E112" t="s">
-        <v>186</v>
-      </c>
-      <c r="H112">
-        <v>1</v>
+        <v>182</v>
+      </c>
+      <c r="F112">
+        <v>0.99</v>
       </c>
       <c r="I112">
-        <v>0.62</v>
+        <v>0.72</v>
       </c>
       <c r="J112">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="K112">
         <v>2030</v>
       </c>
       <c r="L112">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="M112">
         <v>0</v>
@@ -7673,86 +7676,86 @@
         <v>0</v>
       </c>
       <c r="P112">
-        <v>1</v>
+        <v>0.88300000000000001</v>
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="C113" t="s">
-        <v>178</v>
-      </c>
-      <c r="D113" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E113" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="F113">
-        <v>0.99</v>
+        <v>1</v>
+      </c>
+      <c r="G113">
+        <v>1</v>
       </c>
       <c r="I113">
-        <v>0.72</v>
+        <v>0.59</v>
       </c>
       <c r="J113">
         <v>2014</v>
       </c>
       <c r="K113">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="L113">
         <v>2016</v>
       </c>
       <c r="M113">
-        <v>0</v>
+        <v>4253357.6841606703</v>
       </c>
       <c r="N113">
-        <v>0</v>
+        <v>5127493.4858393297</v>
       </c>
       <c r="P113">
-        <v>0.88300000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C114" t="s">
-        <v>180</v>
+        <v>178</v>
+      </c>
+      <c r="D114" t="s">
+        <v>177</v>
       </c>
       <c r="E114" t="s">
-        <v>173</v>
-      </c>
-      <c r="F114">
-        <v>1</v>
-      </c>
-      <c r="G114">
+        <v>186</v>
+      </c>
+      <c r="H114">
         <v>1</v>
       </c>
       <c r="I114">
-        <v>0.59</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="J114">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="K114">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="L114">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="M114">
-        <v>4253357.6841606703</v>
+        <v>0</v>
       </c>
       <c r="N114">
-        <v>5127493.4858393297</v>
+        <v>0</v>
       </c>
       <c r="P114">
         <v>1</v>
@@ -7760,34 +7763,34 @@
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B115" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C115" t="s">
-        <v>178</v>
-      </c>
-      <c r="D115" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E115" t="s">
-        <v>186</v>
-      </c>
-      <c r="H115">
-        <v>1</v>
+        <v>173</v>
+      </c>
+      <c r="F115">
+        <v>0.99</v>
+      </c>
+      <c r="G115">
+        <v>0.99</v>
       </c>
       <c r="I115">
-        <v>0.56000000000000005</v>
+        <v>0.37</v>
       </c>
       <c r="J115">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="K115">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="L115">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="M115">
         <v>0</v>
@@ -7796,15 +7799,15 @@
         <v>0</v>
       </c>
       <c r="P115">
-        <v>1</v>
+        <v>1.52E-2</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B116" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C116" t="s">
         <v>180</v>
@@ -7813,13 +7816,13 @@
         <v>173</v>
       </c>
       <c r="F116">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="G116">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="I116">
-        <v>0.37</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="J116">
         <v>2017</v>
@@ -7837,15 +7840,15 @@
         <v>0</v>
       </c>
       <c r="P116">
-        <v>1.52E-2</v>
+        <v>1.24E-2</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B117" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C117" t="s">
         <v>180</v>
@@ -7854,19 +7857,19 @@
         <v>173</v>
       </c>
       <c r="F117">
-        <v>1</v>
+        <v>0.66839999999999999</v>
       </c>
       <c r="G117">
-        <v>1</v>
+        <v>0.66839999999999999</v>
       </c>
       <c r="I117">
-        <v>0.35000000000000003</v>
+        <v>0.81</v>
       </c>
       <c r="J117">
         <v>2017</v>
       </c>
       <c r="K117">
-        <v>2018</v>
+        <v>2027</v>
       </c>
       <c r="L117">
         <v>2018</v>
@@ -7878,30 +7881,33 @@
         <v>0</v>
       </c>
       <c r="P117">
-        <v>1.24E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B118" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C118" t="s">
-        <v>180</v>
+        <v>178</v>
+      </c>
+      <c r="D118" t="s">
+        <v>177</v>
       </c>
       <c r="E118" t="s">
         <v>173</v>
       </c>
       <c r="F118">
-        <v>0.66839999999999999</v>
+        <v>0.2024</v>
       </c>
       <c r="G118">
-        <v>0.66839999999999999</v>
+        <v>0.2024</v>
       </c>
       <c r="I118">
-        <v>0.81</v>
+        <v>0.67</v>
       </c>
       <c r="J118">
         <v>2017</v>
@@ -7919,7 +7925,7 @@
         <v>0</v>
       </c>
       <c r="P118">
-        <v>0.25</v>
+        <v>0.154</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
@@ -7939,19 +7945,19 @@
         <v>173</v>
       </c>
       <c r="F119">
-        <v>0.2024</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="G119">
-        <v>0.2024</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="I119">
-        <v>0.67</v>
+        <v>0.2</v>
       </c>
       <c r="J119">
         <v>2017</v>
       </c>
       <c r="K119">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="L119">
         <v>2018</v>
@@ -7963,7 +7969,7 @@
         <v>0</v>
       </c>
       <c r="P119">
-        <v>0.154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
@@ -7974,31 +7980,28 @@
         <v>115</v>
       </c>
       <c r="C120" t="s">
-        <v>178</v>
-      </c>
-      <c r="D120" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E120" t="s">
         <v>173</v>
       </c>
       <c r="F120">
-        <v>0.66900000000000004</v>
+        <v>1</v>
       </c>
       <c r="G120">
-        <v>0.66900000000000004</v>
+        <v>1</v>
       </c>
       <c r="I120">
-        <v>0.2</v>
+        <v>0.9</v>
       </c>
       <c r="J120">
-        <v>2017</v>
+        <v>2009</v>
       </c>
       <c r="K120">
-        <v>2025</v>
+        <v>2020</v>
       </c>
       <c r="L120">
-        <v>2018</v>
+        <v>2010</v>
       </c>
       <c r="M120">
         <v>0</v>
@@ -8007,7 +8010,7 @@
         <v>0</v>
       </c>
       <c r="P120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
@@ -8018,19 +8021,22 @@
         <v>115</v>
       </c>
       <c r="C121" t="s">
-        <v>180</v>
+        <v>178</v>
+      </c>
+      <c r="D121" t="s">
+        <v>184</v>
       </c>
       <c r="E121" t="s">
         <v>173</v>
       </c>
       <c r="F121">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="G121">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="I121">
-        <v>0.9</v>
+        <v>0.46</v>
       </c>
       <c r="J121">
         <v>2009</v>
@@ -8042,56 +8048,12 @@
         <v>2010</v>
       </c>
       <c r="M121">
-        <v>0</v>
+        <v>65465.244156436005</v>
       </c>
       <c r="N121">
-        <v>0</v>
+        <v>2292.7558435639962</v>
       </c>
       <c r="P121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>114</v>
-      </c>
-      <c r="B122" t="s">
-        <v>115</v>
-      </c>
-      <c r="C122" t="s">
-        <v>178</v>
-      </c>
-      <c r="D122" t="s">
-        <v>184</v>
-      </c>
-      <c r="E122" t="s">
-        <v>173</v>
-      </c>
-      <c r="F122">
-        <v>0.6</v>
-      </c>
-      <c r="G122">
-        <v>0.6</v>
-      </c>
-      <c r="I122">
-        <v>0.46</v>
-      </c>
-      <c r="J122">
-        <v>2009</v>
-      </c>
-      <c r="K122">
-        <v>2020</v>
-      </c>
-      <c r="L122">
-        <v>2010</v>
-      </c>
-      <c r="M122">
-        <v>65465.244156436005</v>
-      </c>
-      <c r="N122">
-        <v>2292.7558435639962</v>
-      </c>
-      <c r="P122">
         <v>0.61</v>
       </c>
     </row>

</xml_diff>